<commit_message>
Implemented the block change event handler
</commit_message>
<xml_diff>
--- a/ClientBoundPacketSupport.xlsx
+++ b/ClientBoundPacketSupport.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="94">
   <si>
     <t>Packet</t>
   </si>
@@ -715,7 +715,7 @@
   <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +820,9 @@
       <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="5" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">

</xml_diff>

<commit_message>
Multi block change handler implementation
</commit_message>
<xml_diff>
--- a/ClientBoundPacketSupport.xlsx
+++ b/ClientBoundPacketSupport.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="95">
   <si>
     <t>Packet</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>hardcoded 24k days</t>
+  </si>
+  <si>
+    <t>Full (not tested)</t>
   </si>
 </sst>
 </file>
@@ -337,7 +340,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,6 +371,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -390,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -398,6 +407,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -715,7 +725,7 @@
   <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,8 +771,8 @@
         <v>24</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="H4" s="6" t="s">
-        <v>92</v>
+      <c r="H4" s="7" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -770,8 +780,8 @@
         <v>22</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="H5" s="5" t="s">
-        <v>83</v>
+      <c r="H5" s="6" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -779,6 +789,9 @@
         <v>21</v>
       </c>
       <c r="B6" s="2"/>
+      <c r="H6" s="5" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -852,7 +865,9 @@
       <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="7" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">

</xml_diff>

<commit_message>
Added the test implementation status matrix
</commit_message>
<xml_diff>
--- a/ClientBoundPacketSupport.xlsx
+++ b/ClientBoundPacketSupport.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
   <si>
     <t>Packet</t>
   </si>
@@ -399,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -408,6 +408,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -724,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F61166AD-D362-44F9-B5F9-2A33564FFD9F}">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,8 +867,8 @@
       <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>94</v>
+      <c r="B18" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1271,18 +1273,14 @@
         <v>86</v>
       </c>
       <c r="B82" s="2"/>
-      <c r="H82" s="3" t="s">
-        <v>84</v>
-      </c>
+      <c r="H82" s="8"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>87</v>
       </c>
       <c r="B83" s="2"/>
-      <c r="H83" s="4" t="s">
-        <v>82</v>
-      </c>
+      <c r="H83" s="9"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
@@ -1291,18 +1289,14 @@
       <c r="B84" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H84" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="H84" s="9"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>89</v>
       </c>
       <c r="B85" s="2"/>
-      <c r="H85" s="5" t="s">
-        <v>83</v>
-      </c>
+      <c r="H85" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implemented the set xp packet handler and changed agetime ticks to unsigned longs
</commit_message>
<xml_diff>
--- a/ClientBoundPacketSupport.xlsx
+++ b/ClientBoundPacketSupport.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="101">
   <si>
     <t>Packet</t>
   </si>
@@ -306,10 +306,28 @@
     <t>Full (no validation)</t>
   </si>
   <si>
-    <t>hardcoded 24k days</t>
-  </si>
-  <si>
     <t>Full (not tested)</t>
+  </si>
+  <si>
+    <t>Unit tests</t>
+  </si>
+  <si>
+    <t>System tests</t>
+  </si>
+  <si>
+    <t>Impl  status</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>system</t>
+  </si>
+  <si>
+    <t>Happy</t>
+  </si>
+  <si>
+    <t>longs instead of ulongs</t>
   </si>
 </sst>
 </file>
@@ -399,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -410,6 +428,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -724,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F61166AD-D362-44F9-B5F9-2A33564FFD9F}">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,22 +756,43 @@
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="44.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -758,8 +800,14 @@
       <c r="H2" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -767,17 +815,29 @@
       <c r="H3" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="2"/>
       <c r="H4" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -785,8 +845,11 @@
       <c r="H5" s="6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -795,468 +858,518 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F37" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F49" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
       <c r="B63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="2"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68" s="2"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
       <c r="B69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D73" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D73" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F73" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
       <c r="B74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>79</v>
       </c>
       <c r="B79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -1288,6 +1401,12 @@
       </c>
       <c r="B84" s="6" t="s">
         <v>92</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="H84" s="9"/>
     </row>

</xml_diff>

<commit_message>
Implemented entity yaw and pitch
</commit_message>
<xml_diff>
--- a/ClientBoundPacketSupport.xlsx
+++ b/ClientBoundPacketSupport.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="103">
   <si>
     <t>Packet</t>
   </si>
@@ -297,9 +297,6 @@
     <t>set compression  (login)</t>
   </si>
   <si>
-    <t>look ignored, no reply</t>
-  </si>
-  <si>
     <t>world/server properties and gamemode ignored</t>
   </si>
   <si>
@@ -315,9 +312,6 @@
     <t>System tests</t>
   </si>
   <si>
-    <t>Impl  status</t>
-  </si>
-  <si>
     <t>unit</t>
   </si>
   <si>
@@ -328,6 +322,18 @@
   </si>
   <si>
     <t>longs instead of ulongs</t>
+  </si>
+  <si>
+    <t>Side effects</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>no reply</t>
   </si>
 </sst>
 </file>
@@ -745,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F61166AD-D362-44F9-B5F9-2A33564FFD9F}">
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,143 +764,157 @@
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="44.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="44.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L1" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="H2" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="J2" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="H3" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="J3" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="H4" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="H5" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="H6" s="5" t="s">
+      <c r="J6" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -907,32 +927,35 @@
       <c r="E13" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F13" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -945,97 +968,100 @@
       <c r="E18" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>84</v>
@@ -1043,13 +1069,16 @@
       <c r="E33" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>84</v>
@@ -1057,20 +1086,23 @@
       <c r="E34" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1083,77 +1115,80 @@
       <c r="E37" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F37" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1166,107 +1201,110 @@
       <c r="E49" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53" s="2"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56" s="2"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62" s="2"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
       <c r="B63" s="2"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -1279,44 +1317,47 @@
       <c r="E66" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F66" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67" s="2"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68" s="2"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
       <c r="B69" s="2"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -1324,83 +1365,86 @@
         <v>83</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F73" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F73" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G73" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
       <c r="B74" s="2"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>79</v>
       </c>
       <c r="B79" s="2"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
       <c r="B80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>
       <c r="B81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>86</v>
       </c>
       <c r="B82" s="2"/>
-      <c r="H82" s="8"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J82" s="8"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>87</v>
       </c>
       <c r="B83" s="2"/>
-      <c r="H83" s="9"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J83" s="9"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>88</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>84</v>
@@ -1408,14 +1452,17 @@
       <c r="E84" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H84" s="9"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F84" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J84" s="9"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>89</v>
       </c>
       <c r="B85" s="2"/>
-      <c r="H85" s="9"/>
+      <c r="J85" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added support for reply packets
</commit_message>
<xml_diff>
--- a/ClientBoundPacketSupport.xlsx
+++ b/ClientBoundPacketSupport.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="103">
   <si>
     <t>Packet</t>
   </si>
@@ -333,7 +333,7 @@
     <t>Implementation</t>
   </si>
   <si>
-    <t>no reply</t>
+    <t>no uuid, no velocity, no metadata, no validation</t>
   </si>
 </sst>
 </file>
@@ -754,7 +754,7 @@
   <dimension ref="A1:M85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +861,21 @@
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" t="s">
+        <v>102</v>
+      </c>
       <c r="J5" s="6" t="s">
         <v>91</v>
       </c>
@@ -1069,8 +1083,8 @@
       <c r="E33" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F33" s="4" t="s">
-        <v>100</v>
+      <c r="F33" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1188,12 +1202,12 @@
       </c>
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>82</v>
+      <c r="B49" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>84</v>
@@ -1204,95 +1218,92 @@
       <c r="F49" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G49" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53" s="2"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56" s="2"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62" s="2"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
       <c r="B63" s="2"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Updated the packet support matrix
</commit_message>
<xml_diff>
--- a/ClientBoundPacketSupport.xlsx
+++ b/ClientBoundPacketSupport.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="106">
   <si>
     <t>Packet</t>
   </si>
@@ -333,7 +333,16 @@
     <t>Implementation</t>
   </si>
   <si>
-    <t>no uuid, no velocity, no metadata, no validation</t>
+    <t>Ignored</t>
+  </si>
+  <si>
+    <t>no uuid, no metadata, no validation</t>
+  </si>
+  <si>
+    <t>no metadata, no validation, creates iplayer</t>
+  </si>
+  <si>
+    <t>no food, no saturation</t>
   </si>
 </sst>
 </file>
@@ -751,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F61166AD-D362-44F9-B5F9-2A33564FFD9F}">
-  <dimension ref="A1:M85"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,6 +865,9 @@
       <c r="L4" s="12" t="s">
         <v>97</v>
       </c>
+      <c r="M4" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -874,7 +886,7 @@
         <v>84</v>
       </c>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>91</v>
@@ -887,7 +899,21 @@
       <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" t="s">
+        <v>104</v>
+      </c>
       <c r="J6" s="5" t="s">
         <v>83</v>
       </c>
@@ -1074,8 +1100,8 @@
       <c r="A33" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>91</v>
+      <c r="B33" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>84</v>
@@ -1152,19 +1178,52 @@
       <c r="A40" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="2"/>
+      <c r="B40" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="2"/>
+      <c r="B41" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1336,7 +1395,21 @@
       <c r="A67" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="2"/>
+      <c r="B67" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G67" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
@@ -1416,7 +1489,18 @@
       <c r="A78" t="s">
         <v>78</v>
       </c>
-      <c r="B78" s="2"/>
+      <c r="B78" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
@@ -1437,43 +1521,45 @@
       <c r="B81" s="2"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>86</v>
-      </c>
-      <c r="B82" s="2"/>
       <c r="J82" s="8"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B83" s="2"/>
       <c r="J83" s="9"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>88</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>84</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B84" s="2"/>
       <c r="J84" s="9"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>88</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F85" t="s">
+        <v>102</v>
+      </c>
+      <c r="J85" s="9"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>89</v>
       </c>
-      <c r="B85" s="2"/>
-      <c r="J85" s="9"/>
+      <c r="B86" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>